<commit_message>
Modified DB + all markers queries done
</commit_message>
<xml_diff>
--- a/data_backend/resources/domain_data/data_annotation.xlsx
+++ b/data_backend/resources/domain_data/data_annotation.xlsx
@@ -20,20 +20,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t xml:space="preserve">annotation_id</t>
   </si>
   <si>
+    <t xml:space="preserve">segment_type</t>
+  </si>
+  <si>
     <t xml:space="preserve">annotation_name</t>
   </si>
   <si>
     <t xml:space="preserve">annotation_type</t>
   </si>
   <si>
-    <t xml:space="preserve">reference_id</t>
-  </si>
-  <si>
     <t xml:space="preserve">PB2</t>
   </si>
   <si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">PA-X</t>
   </si>
   <si>
+    <t xml:space="preserve">HA</t>
+  </si>
+  <si>
     <t xml:space="preserve">HA1</t>
   </si>
   <si>
@@ -61,10 +64,16 @@
     <t xml:space="preserve">NA</t>
   </si>
   <si>
+    <t xml:space="preserve">MP</t>
+  </si>
+  <si>
     <t xml:space="preserve">M1</t>
   </si>
   <si>
     <t xml:space="preserve">M2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NS</t>
   </si>
   <si>
     <t xml:space="preserve">NS-1</t>
@@ -362,7 +371,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.890625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -391,13 +400,13 @@
       <c r="A2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="n">
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="F2" s="2"/>
@@ -406,14 +415,14 @@
       <c r="A3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>1</v>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -421,14 +430,14 @@
       <c r="A4" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>1</v>
+      <c r="D4" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -436,14 +445,14 @@
       <c r="A5" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>2</v>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -451,14 +460,14 @@
       <c r="A6" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>2</v>
+      <c r="D6" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -466,14 +475,14 @@
       <c r="A7" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>3</v>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -481,14 +490,14 @@
       <c r="A8" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>3</v>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -496,14 +505,14 @@
       <c r="A9" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>4</v>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -511,14 +520,14 @@
       <c r="A10" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>5</v>
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -526,14 +535,14 @@
       <c r="A11" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>6</v>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -541,14 +550,14 @@
       <c r="A12" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>6</v>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -556,14 +565,14 @@
       <c r="A13" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>7</v>
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -571,14 +580,14 @@
       <c r="A14" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="n">
-        <v>7</v>
+      <c r="B14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="F14" s="2"/>
     </row>

</xml_diff>

<commit_message>
Changed annotations to include literature cds
</commit_message>
<xml_diff>
--- a/data_backend/resources/domain_data/data_annotation.xlsx
+++ b/data_backend/resources/domain_data/data_annotation.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t xml:space="preserve">annotation_id</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">annotation_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">annotation_type</t>
   </si>
   <si>
     <t xml:space="preserve">PB2</t>
@@ -368,18 +365,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.890625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="25.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16382" min="5" style="1" width="8.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="25.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16381" min="4" style="1" width="8.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="1" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -392,204 +389,174 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>